<commit_message>
Added learning rate decrease toggle, weight decay options and total ETA.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,16 @@
           <t>Total training time</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Gamma</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Weight decay</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -582,6 +592,8 @@
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -645,6 +657,8 @@
         </is>
       </c>
       <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -708,6 +722,8 @@
         </is>
       </c>
       <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -771,6 +787,8 @@
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -834,6 +852,8 @@
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -897,6 +917,8 @@
         </is>
       </c>
       <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -960,6 +982,8 @@
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1023,6 +1047,8 @@
         </is>
       </c>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1088,6 +1114,8 @@
       <c r="Q10" t="n">
         <v>1374.856968400014</v>
       </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1153,6 +1181,8 @@
       <c r="Q11" t="n">
         <v>1377.945881299998</v>
       </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1218,6 +1248,8 @@
       <c r="Q12" t="n">
         <v>1374.454556000019</v>
       </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1283,6 +1315,8 @@
       <c r="Q13" t="n">
         <v>1371.926769800015</v>
       </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1348,6 +1382,8 @@
       <c r="Q14" t="n">
         <v>1372.048912300001</v>
       </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1413,6 +1449,8 @@
       <c r="Q15" t="n">
         <v>1378.138338899989</v>
       </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1478,6 +1516,8 @@
       <c r="Q16" t="n">
         <v>1377.46533599999</v>
       </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1543,6 +1583,8 @@
       <c r="Q17" t="n">
         <v>24.39485630000001</v>
       </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1608,6 +1650,8 @@
       <c r="Q18" t="n">
         <v>19.145033</v>
       </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1673,6 +1717,8 @@
       <c r="Q19" t="n">
         <v>1100.843712800001</v>
       </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1738,6 +1784,8 @@
       <c r="Q20" t="n">
         <v>553.3486225000015</v>
       </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1803,6 +1851,8 @@
       <c r="Q21" t="n">
         <v>534.5941934999937</v>
       </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1867,6 +1917,221 @@
       </c>
       <c r="Q22" t="n">
         <v>1108.301104900009</v>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-1-4 16:44:33</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" t="n">
+        <v>64</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>SGD</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="H23" t="n">
+        <v>32</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1.1581</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1.1581</v>
+      </c>
+      <c r="K23" t="n">
+        <v>56.8985</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>4</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>256.1767744999961</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-1-4 16:53:8</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>20</v>
+      </c>
+      <c r="C24" t="n">
+        <v>64</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>SGD</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="H24" t="n">
+        <v>32</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1.2979</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.1205</v>
+      </c>
+      <c r="K24" t="n">
+        <v>58.5426</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>4</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>249.4619421000061</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-1-4 17:42:41</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>20</v>
+      </c>
+      <c r="C25" t="n">
+        <v>64</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SGD</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="H25" t="n">
+        <v>32</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1.2513</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.1665</v>
+      </c>
+      <c r="K25" t="n">
+        <v>57.5952</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>4</v>
+      </c>
+      <c r="O25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>251.8056318999988</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New models and data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,15 +529,25 @@
           <t>Weight decay</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Scheduler</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Min. LR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-1-3 22:17:58</t>
+          <t>2024-1-4 20:39:23</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
         <v>64</v>
@@ -547,7 +557,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -556,19 +566,19 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>12</v>
+        <v>18.5</v>
       </c>
       <c r="H2" t="n">
         <v>32</v>
       </c>
       <c r="I2" t="n">
-        <v>1.2655</v>
+        <v>1.7122</v>
       </c>
       <c r="J2" t="n">
-        <v>1.2655</v>
+        <v>1.0878</v>
       </c>
       <c r="K2" t="n">
-        <v>42.774</v>
+        <v>25.1315</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -591,18 +601,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="Q2" t="n">
+        <v>370.6461947000134</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-1-3 22:20:30</t>
+          <t>2024-1-4 20:39:24</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
         <v>64</v>
@@ -612,7 +636,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -621,19 +645,19 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>12.2</v>
+        <v>18.5</v>
       </c>
       <c r="H3" t="n">
         <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>1.5613</v>
+        <v>1.8061</v>
       </c>
       <c r="J3" t="n">
-        <v>1.3178</v>
+        <v>1.7311</v>
       </c>
       <c r="K3" t="n">
-        <v>41.9485</v>
+        <v>25.1315</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -656,18 +680,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="Q3" t="n">
+        <v>369.7798029000114</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-1-3 22:24:14</t>
+          <t>2024-1-4 20:39:28</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
         <v>64</v>
@@ -677,7 +715,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -686,19 +724,19 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>12.2</v>
+        <v>18.6</v>
       </c>
       <c r="H4" t="n">
         <v>32</v>
       </c>
       <c r="I4" t="n">
-        <v>1.5382</v>
+        <v>1.9109</v>
       </c>
       <c r="J4" t="n">
-        <v>1.5382</v>
+        <v>1.0383</v>
       </c>
       <c r="K4" t="n">
-        <v>43.5926</v>
+        <v>25.1315</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -721,18 +759,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="Q4" t="n">
+        <v>371.8065964999987</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-1-3 22:28:18</t>
+          <t>2024-1-4 20:39:32</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
         <v>64</v>
@@ -742,7 +794,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -751,19 +803,19 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>12</v>
+        <v>18.7</v>
       </c>
       <c r="H5" t="n">
         <v>32</v>
       </c>
       <c r="I5" t="n">
-        <v>1.298</v>
+        <v>1.7681</v>
       </c>
       <c r="J5" t="n">
-        <v>1.298</v>
+        <v>1.1081</v>
       </c>
       <c r="K5" t="n">
-        <v>43.3488</v>
+        <v>25.1315</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -786,18 +838,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="Q5" t="n">
+        <v>373.5626463999797</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-1-3 22:31:18</t>
+          <t>2024-1-4 20:39:35</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C6" t="n">
         <v>64</v>
@@ -807,7 +873,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -816,19 +882,19 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>12.2</v>
+        <v>18.7</v>
       </c>
       <c r="H6" t="n">
         <v>32</v>
       </c>
       <c r="I6" t="n">
-        <v>1.4345</v>
+        <v>1.7477</v>
       </c>
       <c r="J6" t="n">
-        <v>1.4345</v>
+        <v>1.7206</v>
       </c>
       <c r="K6" t="n">
-        <v>43.6135</v>
+        <v>25.1315</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -851,18 +917,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+      <c r="Q6" t="n">
+        <v>373.6902389000097</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-1-3 22:33:51</t>
+          <t>2024-1-4 20:39:36</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C7" t="n">
         <v>64</v>
@@ -872,7 +952,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -881,19 +961,19 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>12.1</v>
+        <v>18.7</v>
       </c>
       <c r="H7" t="n">
         <v>32</v>
       </c>
       <c r="I7" t="n">
-        <v>1.4563</v>
+        <v>1.8374</v>
       </c>
       <c r="J7" t="n">
-        <v>1.4563</v>
+        <v>1.3988</v>
       </c>
       <c r="K7" t="n">
-        <v>43.1885</v>
+        <v>25.1315</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -916,18 +996,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="Q7" t="n">
+        <v>373.3237019000153</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-1-3 22:42:10</t>
+          <t>2024-1-4 20:39:41</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C8" t="n">
         <v>64</v>
@@ -937,7 +1031,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -946,19 +1040,19 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>12.3</v>
+        <v>18.6</v>
       </c>
       <c r="H8" t="n">
         <v>32</v>
       </c>
       <c r="I8" t="n">
-        <v>1.6126</v>
+        <v>1.9666</v>
       </c>
       <c r="J8" t="n">
-        <v>1.5489</v>
+        <v>1.7187</v>
       </c>
       <c r="K8" t="n">
-        <v>43.4916</v>
+        <v>25.1315</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -981,18 +1075,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="Q8" t="n">
+        <v>372.541074599998</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-1-3 23:49:12</t>
+          <t>2024-1-4 20:39:42</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C9" t="n">
         <v>64</v>
@@ -1002,7 +1110,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1011,19 +1119,19 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>14.4</v>
+        <v>18.8</v>
       </c>
       <c r="H9" t="n">
         <v>32</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5636</v>
+        <v>1.7903</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2941</v>
+        <v>1.1538</v>
       </c>
       <c r="K9" t="n">
-        <v>89.101</v>
+        <v>25.1315</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1046,18 +1154,32 @@
           <t>Stationær</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="Q9" t="n">
+        <v>376.7640408000007</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:17</t>
+          <t>2024-1-4 20:39:44</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C10" t="n">
         <v>64</v>
@@ -1067,7 +1189,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1076,19 +1198,19 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>13.7</v>
+        <v>18.6</v>
       </c>
       <c r="H10" t="n">
         <v>32</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6725</v>
+        <v>1.7859</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3469</v>
+        <v>1.6927</v>
       </c>
       <c r="K10" t="n">
-        <v>87.27930000000001</v>
+        <v>25.1315</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1112,19 +1234,31 @@
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>1374.856968400014</v>
-      </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+        <v>372.0865585000065</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:22</t>
+          <t>2024-1-4 20:39:45</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C11" t="n">
         <v>64</v>
@@ -1134,7 +1268,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1143,19 +1277,19 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>13.8</v>
+        <v>18.6</v>
       </c>
       <c r="H11" t="n">
         <v>32</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6863</v>
+        <v>1.8096</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2965</v>
+        <v>1.7351</v>
       </c>
       <c r="K11" t="n">
-        <v>87.20610000000001</v>
+        <v>25.1315</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1179,19 +1313,31 @@
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>1377.945881299998</v>
-      </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+        <v>371.3381179999924</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:27</t>
+          <t>2024-1-4 20:45:55</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
         <v>64</v>
@@ -1201,7 +1347,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1210,19 +1356,19 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>13.7</v>
+        <v>18.4</v>
       </c>
       <c r="H12" t="n">
         <v>32</v>
       </c>
       <c r="I12" t="n">
-        <v>0.8611</v>
+        <v>1.6599</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2981</v>
+        <v>1.6599</v>
       </c>
       <c r="K12" t="n">
-        <v>87.0946</v>
+        <v>25.1315</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1246,19 +1392,31 @@
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>1374.454556000019</v>
-      </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+        <v>367.8006071999989</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:35</t>
+          <t>2024-1-4 20:45:58</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C13" t="n">
         <v>64</v>
@@ -1268,7 +1426,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1277,19 +1435,19 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>13.7</v>
+        <v>18.3</v>
       </c>
       <c r="H13" t="n">
         <v>32</v>
       </c>
       <c r="I13" t="n">
-        <v>0.5886</v>
+        <v>1.824</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3802</v>
+        <v>1.7302</v>
       </c>
       <c r="K13" t="n">
-        <v>88.43219999999999</v>
+        <v>25.1315</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1313,19 +1471,31 @@
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>1371.926769800015</v>
-      </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+        <v>366.5414939000111</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:36</t>
+          <t>2024-1-4 20:45:58</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C14" t="n">
         <v>64</v>
@@ -1335,7 +1505,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1344,19 +1514,19 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>13.7</v>
+        <v>18.5</v>
       </c>
       <c r="H14" t="n">
         <v>32</v>
       </c>
       <c r="I14" t="n">
-        <v>0.875</v>
+        <v>1.7611</v>
       </c>
       <c r="J14" t="n">
-        <v>0.368</v>
+        <v>1.7077</v>
       </c>
       <c r="K14" t="n">
-        <v>87.20959999999999</v>
+        <v>25.1315</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1380,19 +1550,31 @@
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>1372.048912300001</v>
-      </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+        <v>369.3373302999971</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:38</t>
+          <t>2024-1-4 20:46:3</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C15" t="n">
         <v>64</v>
@@ -1402,7 +1584,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1411,19 +1593,19 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>13.8</v>
+        <v>18.3</v>
       </c>
       <c r="H15" t="n">
         <v>32</v>
       </c>
       <c r="I15" t="n">
-        <v>0.6145</v>
+        <v>1.9143</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3914</v>
+        <v>1.7187</v>
       </c>
       <c r="K15" t="n">
-        <v>87.5823</v>
+        <v>25.1315</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1447,19 +1629,31 @@
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>1378.138338899989</v>
-      </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+        <v>366.9219385999968</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-1-4 0:13:39</t>
+          <t>2024-1-4 20:46:4</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C16" t="n">
         <v>64</v>
@@ -1469,7 +1663,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1478,19 +1672,19 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>13.8</v>
+        <v>18.3</v>
       </c>
       <c r="H16" t="n">
         <v>32</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6299</v>
+        <v>1.8569</v>
       </c>
       <c r="J16" t="n">
-        <v>0.353</v>
+        <v>1.1807</v>
       </c>
       <c r="K16" t="n">
-        <v>88.4148</v>
+        <v>25.1315</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1514,19 +1708,31 @@
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>1377.46533599999</v>
-      </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+        <v>366.7385061999885</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-1-4 9:28:46</t>
+          <t>2024-1-4 20:46:7</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C17" t="n">
         <v>64</v>
@@ -1536,7 +1742,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1545,19 +1751,19 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>24.4</v>
+        <v>18.3</v>
       </c>
       <c r="H17" t="n">
         <v>32</v>
       </c>
       <c r="I17" t="n">
-        <v>1.5311</v>
+        <v>1.8123</v>
       </c>
       <c r="J17" t="n">
-        <v>1.5311</v>
+        <v>1.7485</v>
       </c>
       <c r="K17" t="n">
-        <v>36.6888</v>
+        <v>25.1315</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1581,19 +1787,31 @@
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>24.39485630000001</v>
-      </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+        <v>366.7254802999887</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-1-4 9:31:35</t>
+          <t>2024-1-4 20:46:13</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C18" t="n">
         <v>64</v>
@@ -1603,7 +1821,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1612,19 +1830,19 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>19.1</v>
+        <v>18.4</v>
       </c>
       <c r="H18" t="n">
         <v>32</v>
       </c>
       <c r="I18" t="n">
-        <v>1.5769</v>
+        <v>1.8246</v>
       </c>
       <c r="J18" t="n">
-        <v>1.5769</v>
+        <v>1.1734</v>
       </c>
       <c r="K18" t="n">
-        <v>37.9602</v>
+        <v>25.1315</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1648,29 +1866,41 @@
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>19.145033</v>
-      </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+        <v>367.2518276000046</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-1-4 10:50:30</t>
+          <t>2024-1-4 20:46:14</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C19" t="n">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D19" t="n">
         <v>0.01</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1679,19 +1909,19 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>11</v>
+        <v>18.5</v>
       </c>
       <c r="H19" t="n">
         <v>32</v>
       </c>
       <c r="I19" t="n">
-        <v>0.8203</v>
+        <v>1.7414</v>
       </c>
       <c r="J19" t="n">
-        <v>0.178</v>
+        <v>1.7001</v>
       </c>
       <c r="K19" t="n">
-        <v>93.1032</v>
+        <v>25.1315</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1715,29 +1945,41 @@
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>1100.843712800001</v>
-      </c>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+        <v>369.8789915000016</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-1-4 11:15:24</t>
+          <t>2024-1-4 20:46:18</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D20" t="n">
         <v>0.01</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1746,19 +1988,19 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>11.1</v>
+        <v>18.5</v>
       </c>
       <c r="H20" t="n">
         <v>32</v>
       </c>
       <c r="I20" t="n">
-        <v>0.596</v>
+        <v>1.8162</v>
       </c>
       <c r="J20" t="n">
-        <v>0.4173</v>
+        <v>1.7087</v>
       </c>
       <c r="K20" t="n">
-        <v>89.7384</v>
+        <v>25.1315</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1782,29 +2024,41 @@
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>553.3486225000015</v>
-      </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+        <v>370.1409788999808</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-1-4 12:24:50</t>
+          <t>2024-1-4 20:46:19</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="D21" t="n">
         <v>0.01</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1813,19 +2067,19 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>10.7</v>
+        <v>18.4</v>
       </c>
       <c r="H21" t="n">
         <v>32</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2889</v>
+        <v>1.7768</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2889</v>
+        <v>1.7233</v>
       </c>
       <c r="K21" t="n">
-        <v>87.4046</v>
+        <v>25.1315</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1849,29 +2103,41 @@
         </is>
       </c>
       <c r="Q21" t="n">
-        <v>534.5941934999937</v>
-      </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+        <v>368.0760812000008</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-1-4 13:7:49</t>
+          <t>2024-1-4 20:52:30</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D22" t="n">
         <v>0.01</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1880,19 +2146,19 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>11.1</v>
+        <v>18.6</v>
       </c>
       <c r="H22" t="n">
         <v>32</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3164</v>
+        <v>1.7921</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2122</v>
+        <v>1.7185</v>
       </c>
       <c r="K22" t="n">
-        <v>92.45529999999999</v>
+        <v>25.1315</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -1916,15 +2182,27 @@
         </is>
       </c>
       <c r="Q22" t="n">
-        <v>1108.301104900009</v>
-      </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+        <v>372.7849623999864</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-1-4 16:44:33</t>
+          <t>2024-1-4 20:52:34</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1934,11 +2212,11 @@
         <v>64</v>
       </c>
       <c r="D23" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1947,19 +2225,19 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>12.8</v>
+        <v>18.6</v>
       </c>
       <c r="H23" t="n">
         <v>32</v>
       </c>
       <c r="I23" t="n">
-        <v>1.1581</v>
+        <v>1.8511</v>
       </c>
       <c r="J23" t="n">
-        <v>1.1581</v>
+        <v>1.2295</v>
       </c>
       <c r="K23" t="n">
-        <v>56.8985</v>
+        <v>25.1315</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -1983,19 +2261,27 @@
         </is>
       </c>
       <c r="Q23" t="n">
-        <v>256.1767744999961</v>
+        <v>372.7298785999737</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
       </c>
       <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024-1-4 16:53:8</t>
+          <t>2024-1-4 20:52:36</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2005,11 +2291,11 @@
         <v>64</v>
       </c>
       <c r="D24" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>ADAM</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2018,19 +2304,19 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>12.5</v>
+        <v>18.6</v>
       </c>
       <c r="H24" t="n">
         <v>32</v>
       </c>
       <c r="I24" t="n">
-        <v>1.2979</v>
+        <v>1.7189</v>
       </c>
       <c r="J24" t="n">
-        <v>1.1205</v>
+        <v>1.6861</v>
       </c>
       <c r="K24" t="n">
-        <v>58.5426</v>
+        <v>25.1315</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -2054,19 +2340,27 @@
         </is>
       </c>
       <c r="Q24" t="n">
-        <v>249.4619421000061</v>
+        <v>372.4233570000069</v>
       </c>
       <c r="R24" t="n">
         <v>0</v>
       </c>
       <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024-1-4 17:42:41</t>
+          <t>2024-1-4 20:52:37</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2076,61 +2370,3212 @@
         <v>64</v>
       </c>
       <c r="D25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H25" t="n">
+        <v>32</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1.7696</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.7137</v>
+      </c>
+      <c r="K25" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>4</v>
+      </c>
+      <c r="O25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>372.1531827999861</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:52:38</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>20</v>
+      </c>
+      <c r="C26" t="n">
+        <v>64</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="H26" t="n">
+        <v>32</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.7998</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.7307</v>
+      </c>
+      <c r="K26" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>4</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>370.7091821999929</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:52:40</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>20</v>
+      </c>
+      <c r="C27" t="n">
+        <v>64</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="H27" t="n">
+        <v>32</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1.8197</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.7012</v>
+      </c>
+      <c r="K27" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>4</v>
+      </c>
+      <c r="O27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>370.9270204000059</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:52:47</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>20</v>
+      </c>
+      <c r="C28" t="n">
+        <v>64</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H28" t="n">
+        <v>32</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1.8051</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1.6565</v>
+      </c>
+      <c r="K28" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>4</v>
+      </c>
+      <c r="O28" t="n">
+        <v>2</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>371.015299799983</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:52:48</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>20</v>
+      </c>
+      <c r="C29" t="n">
+        <v>64</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="H29" t="n">
+        <v>32</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1.9054</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1.3376</v>
+      </c>
+      <c r="K29" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>4</v>
+      </c>
+      <c r="O29" t="n">
+        <v>2</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>370.1616004000171</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:52:53</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>20</v>
+      </c>
+      <c r="C30" t="n">
+        <v>64</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H30" t="n">
+        <v>32</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1.7173</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.6354</v>
+      </c>
+      <c r="K30" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>4</v>
+      </c>
+      <c r="O30" t="n">
+        <v>2</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>371.6832794999937</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:52:56</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>20</v>
+      </c>
+      <c r="C31" t="n">
+        <v>64</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H31" t="n">
+        <v>32</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1.7477</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.1284</v>
+      </c>
+      <c r="K31" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>4</v>
+      </c>
+      <c r="O31" t="n">
+        <v>2</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>372.0355971999816</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:7</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>20</v>
+      </c>
+      <c r="C32" t="n">
+        <v>64</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H32" t="n">
+        <v>32</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1.8094</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1.7029</v>
+      </c>
+      <c r="K32" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>4</v>
+      </c>
+      <c r="O32" t="n">
+        <v>2</v>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>373.4731284999871</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:12</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>20</v>
+      </c>
+      <c r="C33" t="n">
+        <v>64</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H33" t="n">
+        <v>32</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1.7682</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1.6841</v>
+      </c>
+      <c r="K33" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>4</v>
+      </c>
+      <c r="O33" t="n">
+        <v>2</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>374.4399899999989</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:13</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>20</v>
+      </c>
+      <c r="C34" t="n">
+        <v>64</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H34" t="n">
+        <v>32</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1.7803</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1.2082</v>
+      </c>
+      <c r="K34" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>4</v>
+      </c>
+      <c r="O34" t="n">
+        <v>2</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>374.2216514999964</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:14</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>20</v>
+      </c>
+      <c r="C35" t="n">
+        <v>64</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H35" t="n">
+        <v>32</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1.7411</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1.7185</v>
+      </c>
+      <c r="K35" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>4</v>
+      </c>
+      <c r="O35" t="n">
+        <v>2</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q35" t="n">
+        <v>373.1466780000046</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:16</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>20</v>
+      </c>
+      <c r="C36" t="n">
+        <v>64</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H36" t="n">
+        <v>32</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1.9585</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1.682</v>
+      </c>
+      <c r="K36" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>4</v>
+      </c>
+      <c r="O36" t="n">
+        <v>2</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q36" t="n">
+        <v>372.8134187000032</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:18</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>20</v>
+      </c>
+      <c r="C37" t="n">
+        <v>64</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H37" t="n">
+        <v>32</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1.8802</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1.6962</v>
+      </c>
+      <c r="K37" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>4</v>
+      </c>
+      <c r="O37" t="n">
+        <v>2</v>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q37" t="n">
+        <v>372.5105418000167</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:22</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>20</v>
+      </c>
+      <c r="C38" t="n">
+        <v>64</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H38" t="n">
+        <v>32</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1.8039</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1.3727</v>
+      </c>
+      <c r="K38" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>4</v>
+      </c>
+      <c r="O38" t="n">
+        <v>2</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q38" t="n">
+        <v>371.2063561000105</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:26</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>20</v>
+      </c>
+      <c r="C39" t="n">
+        <v>64</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H39" t="n">
+        <v>32</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1.9263</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1.7171</v>
+      </c>
+      <c r="K39" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>4</v>
+      </c>
+      <c r="O39" t="n">
+        <v>2</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q39" t="n">
+        <v>373.0705715000004</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:30</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>20</v>
+      </c>
+      <c r="C40" t="n">
+        <v>64</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H40" t="n">
+        <v>32</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1.8643</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1.2063</v>
+      </c>
+      <c r="K40" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>4</v>
+      </c>
+      <c r="O40" t="n">
+        <v>2</v>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q40" t="n">
+        <v>373.1876866999737</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-1-4 20:59:31</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>20</v>
+      </c>
+      <c r="C41" t="n">
+        <v>64</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="H41" t="n">
+        <v>32</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2.0274</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1.7192</v>
+      </c>
+      <c r="K41" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>4</v>
+      </c>
+      <c r="O41" t="n">
+        <v>2</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q41" t="n">
+        <v>371.5940374999991</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:33:57</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>20</v>
+      </c>
+      <c r="C42" t="n">
+        <v>64</v>
+      </c>
+      <c r="D42" t="n">
         <v>0.001</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>SGD</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>CEL</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>12.6</v>
-      </c>
-      <c r="H25" t="n">
-        <v>32</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1.2513</v>
-      </c>
-      <c r="J25" t="n">
-        <v>1.1665</v>
-      </c>
-      <c r="K25" t="n">
-        <v>57.5952</v>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>FER2013</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>cuda:0</t>
-        </is>
-      </c>
-      <c r="N25" t="n">
-        <v>4</v>
-      </c>
-      <c r="O25" t="n">
-        <v>2</v>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>Stationær</t>
-        </is>
-      </c>
-      <c r="Q25" t="n">
-        <v>251.8056318999988</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" t="n">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="H42" t="n">
+        <v>32</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.1159</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.1017</v>
+      </c>
+      <c r="K42" t="n">
+        <v>96.9173</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>4</v>
+      </c>
+      <c r="O42" t="n">
+        <v>2</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q42" t="n">
+        <v>383.8204586000065</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:1</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>20</v>
+      </c>
+      <c r="C43" t="n">
+        <v>64</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="H43" t="n">
+        <v>32</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.3691</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.1308</v>
+      </c>
+      <c r="K43" t="n">
+        <v>96.4819</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>4</v>
+      </c>
+      <c r="O43" t="n">
+        <v>2</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q43" t="n">
+        <v>385.6173490999936</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:3</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>20</v>
+      </c>
+      <c r="C44" t="n">
+        <v>64</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="H44" t="n">
+        <v>32</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.0419</v>
+      </c>
+      <c r="K44" t="n">
+        <v>96.96259999999999</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>4</v>
+      </c>
+      <c r="O44" t="n">
+        <v>2</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q44" t="n">
+        <v>385.6189726999874</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0</v>
+      </c>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:7</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>20</v>
+      </c>
+      <c r="C45" t="n">
+        <v>64</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="H45" t="n">
+        <v>32</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="K45" t="n">
+        <v>96.3078</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>4</v>
+      </c>
+      <c r="O45" t="n">
+        <v>2</v>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q45" t="n">
+        <v>387.4170694999993</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0</v>
+      </c>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:8</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>20</v>
+      </c>
+      <c r="C46" t="n">
+        <v>64</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="H46" t="n">
+        <v>32</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.2576</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.0419</v>
+      </c>
+      <c r="K46" t="n">
+        <v>96.4192</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>4</v>
+      </c>
+      <c r="O46" t="n">
+        <v>2</v>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q46" t="n">
+        <v>386.5243570000312</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0</v>
+      </c>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:13</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>20</v>
+      </c>
+      <c r="C47" t="n">
+        <v>64</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="H47" t="n">
+        <v>32</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.2545</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.1044</v>
+      </c>
+      <c r="K47" t="n">
+        <v>96.17189999999999</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>4</v>
+      </c>
+      <c r="O47" t="n">
+        <v>2</v>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q47" t="n">
+        <v>388.5180582999747</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0</v>
+      </c>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:15</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>20</v>
+      </c>
+      <c r="C48" t="n">
+        <v>64</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="H48" t="n">
+        <v>32</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.6077</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.0978</v>
+      </c>
+      <c r="K48" t="n">
+        <v>97.49209999999999</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>4</v>
+      </c>
+      <c r="O48" t="n">
+        <v>2</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q48" t="n">
+        <v>388.6524073999826</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0</v>
+      </c>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:16</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>20</v>
+      </c>
+      <c r="C49" t="n">
+        <v>64</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="H49" t="n">
+        <v>32</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.2221</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="K49" t="n">
+        <v>96.0326</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>4</v>
+      </c>
+      <c r="O49" t="n">
+        <v>2</v>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q49" t="n">
+        <v>387.5095757000017</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0</v>
+      </c>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:18</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>20</v>
+      </c>
+      <c r="C50" t="n">
+        <v>64</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="H50" t="n">
+        <v>32</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.2359</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="K50" t="n">
+        <v>96.85120000000001</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>4</v>
+      </c>
+      <c r="O50" t="n">
+        <v>2</v>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q50" t="n">
+        <v>387.098123100026</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0</v>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:34:23</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>20</v>
+      </c>
+      <c r="C51" t="n">
+        <v>64</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="H51" t="n">
+        <v>32</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.2299</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.0853</v>
+      </c>
+      <c r="K51" t="n">
+        <v>96.78149999999999</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>4</v>
+      </c>
+      <c r="O51" t="n">
+        <v>2</v>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q51" t="n">
+        <v>389.5725970000058</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="n">
+        <v>0</v>
+      </c>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:40:40</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>20</v>
+      </c>
+      <c r="C52" t="n">
+        <v>64</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="H52" t="n">
+        <v>32</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.2426</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.0808</v>
+      </c>
+      <c r="K52" t="n">
+        <v>95.6634</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>4</v>
+      </c>
+      <c r="O52" t="n">
+        <v>2</v>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q52" t="n">
+        <v>378.7755820999955</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0</v>
+      </c>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:40:45</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>20</v>
+      </c>
+      <c r="C53" t="n">
+        <v>64</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>19</v>
+      </c>
+      <c r="H53" t="n">
+        <v>32</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.1808</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.1062</v>
+      </c>
+      <c r="K53" t="n">
+        <v>96.2242</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>4</v>
+      </c>
+      <c r="O53" t="n">
+        <v>2</v>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q53" t="n">
+        <v>379.4799841000058</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="n">
+        <v>0</v>
+      </c>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:40:46</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>20</v>
+      </c>
+      <c r="C54" t="n">
+        <v>64</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="H54" t="n">
+        <v>32</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.2687</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.1541</v>
+      </c>
+      <c r="K54" t="n">
+        <v>95.84099999999999</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>4</v>
+      </c>
+      <c r="O54" t="n">
+        <v>2</v>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q54" t="n">
+        <v>378.7031901000082</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0</v>
+      </c>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:40:50</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>20</v>
+      </c>
+      <c r="C55" t="n">
+        <v>64</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="H55" t="n">
+        <v>32</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.0654</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.0618</v>
+      </c>
+      <c r="K55" t="n">
+        <v>96.78149999999999</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>4</v>
+      </c>
+      <c r="O55" t="n">
+        <v>2</v>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q55" t="n">
+        <v>378.8537553999995</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="n">
+        <v>0</v>
+      </c>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:40:52</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>20</v>
+      </c>
+      <c r="C56" t="n">
+        <v>64</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="H56" t="n">
+        <v>32</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.1412</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.1237</v>
+      </c>
+      <c r="K56" t="n">
+        <v>95.1688</v>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>4</v>
+      </c>
+      <c r="O56" t="n">
+        <v>2</v>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q56" t="n">
+        <v>378.6080862000235</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0</v>
+      </c>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:40:57</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>20</v>
+      </c>
+      <c r="C57" t="n">
+        <v>64</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="H57" t="n">
+        <v>32</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.3621</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.0687</v>
+      </c>
+      <c r="K57" t="n">
+        <v>96.29730000000001</v>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>4</v>
+      </c>
+      <c r="O57" t="n">
+        <v>2</v>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q57" t="n">
+        <v>377.8378886999781</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" t="n">
+        <v>0</v>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:8:15</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>20</v>
+      </c>
+      <c r="C58" t="n">
+        <v>64</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="H58" t="n">
+        <v>32</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.1592</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.0342</v>
+      </c>
+      <c r="K58" t="n">
+        <v>95.4474</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>4</v>
+      </c>
+      <c r="O58" t="n">
+        <v>2</v>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q58" t="n">
+        <v>368.9521090999988</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0</v>
+      </c>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:15:45</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>20</v>
+      </c>
+      <c r="C59" t="n">
+        <v>64</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="H59" t="n">
+        <v>32</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.1633</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.1026</v>
+      </c>
+      <c r="K59" t="n">
+        <v>97.2657</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>4</v>
+      </c>
+      <c r="O59" t="n">
+        <v>2</v>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q59" t="n">
+        <v>263.2782270000171</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0</v>
+      </c>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:22:19</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>64</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="H60" t="n">
+        <v>32</v>
+      </c>
+      <c r="I60" t="n">
+        <v>1.8234</v>
+      </c>
+      <c r="J60" t="n">
+        <v>1.8234</v>
+      </c>
+      <c r="K60" t="n">
+        <v>25.438</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>4</v>
+      </c>
+      <c r="O60" t="n">
+        <v>2</v>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q60" t="n">
+        <v>13.60490530000243</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S60" t="n">
+        <v>0</v>
+      </c>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:23:10</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" t="n">
+        <v>64</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="H61" t="n">
+        <v>32</v>
+      </c>
+      <c r="I61" t="n">
+        <v>1.5693</v>
+      </c>
+      <c r="J61" t="n">
+        <v>1.5693</v>
+      </c>
+      <c r="K61" t="n">
+        <v>31.8924</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>4</v>
+      </c>
+      <c r="O61" t="n">
+        <v>2</v>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q61" t="n">
+        <v>13.64818940000259</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S61" t="n">
+        <v>0</v>
+      </c>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:24:20</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>64</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>32</v>
+      </c>
+      <c r="I62" t="n">
+        <v>1.8071</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1.8071</v>
+      </c>
+      <c r="K62" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>4</v>
+      </c>
+      <c r="O62" t="n">
+        <v>2</v>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q62" t="n">
+        <v>13.05898760000127</v>
+      </c>
+      <c r="R62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S62" t="n">
+        <v>0</v>
+      </c>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:25:26</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>64</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="H63" t="n">
+        <v>32</v>
+      </c>
+      <c r="I63" t="n">
+        <v>1.7553</v>
+      </c>
+      <c r="J63" t="n">
+        <v>1.7553</v>
+      </c>
+      <c r="K63" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>4</v>
+      </c>
+      <c r="O63" t="n">
+        <v>2</v>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q63" t="n">
+        <v>12.79654540000047</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S63" t="n">
+        <v>0</v>
+      </c>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:26:9</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="n">
+        <v>64</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="H64" t="n">
+        <v>32</v>
+      </c>
+      <c r="I64" t="n">
+        <v>1.8426</v>
+      </c>
+      <c r="J64" t="n">
+        <v>1.8426</v>
+      </c>
+      <c r="K64" t="n">
+        <v>25.1315</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>4</v>
+      </c>
+      <c r="O64" t="n">
+        <v>2</v>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q64" t="n">
+        <v>13.11443980000331</v>
+      </c>
+      <c r="R64" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:26:41</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="n">
+        <v>64</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="H65" t="n">
+        <v>32</v>
+      </c>
+      <c r="I65" t="n">
+        <v>1.9843</v>
+      </c>
+      <c r="J65" t="n">
+        <v>1.9843</v>
+      </c>
+      <c r="K65" t="n">
+        <v>18.8756</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>4</v>
+      </c>
+      <c r="O65" t="n">
+        <v>2</v>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q65" t="n">
+        <v>13.06263939999917</v>
+      </c>
+      <c r="R65" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S65" t="n">
+        <v>0</v>
+      </c>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:27:31</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>64</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="H66" t="n">
+        <v>32</v>
+      </c>
+      <c r="I66" t="n">
+        <v>1.7497</v>
+      </c>
+      <c r="J66" t="n">
+        <v>1.7497</v>
+      </c>
+      <c r="K66" t="n">
+        <v>36.1942</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>4</v>
+      </c>
+      <c r="O66" t="n">
+        <v>2</v>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q66" t="n">
+        <v>13.19201839999732</v>
+      </c>
+      <c r="R66" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S66" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U66" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New date (remember to change ADAM to SGD)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U86"/>
+  <dimension ref="A1:U96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7070,12 +7070,762 @@
       <c r="S86" t="n">
         <v>0.005</v>
       </c>
-      <c r="T86" t="inlineStr">
+      <c r="T86" t="inlineStr"/>
+      <c r="U86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:14:18</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>20</v>
+      </c>
+      <c r="C87" t="n">
+        <v>64</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="H87" t="n">
+        <v>32</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1.5145</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1.1936</v>
+      </c>
+      <c r="K87" t="n">
+        <v>51.8792</v>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N87" t="n">
+        <v>4</v>
+      </c>
+      <c r="O87" t="n">
+        <v>2</v>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q87" t="n">
+        <v>263.1</v>
+      </c>
+      <c r="R87" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T87" t="inlineStr"/>
+      <c r="U87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:16:24</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>20</v>
+      </c>
+      <c r="C88" t="n">
+        <v>64</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="H88" t="n">
+        <v>32</v>
+      </c>
+      <c r="I88" t="n">
+        <v>1.272</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1.1194</v>
+      </c>
+      <c r="K88" t="n">
+        <v>54.5926</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N88" t="n">
+        <v>4</v>
+      </c>
+      <c r="O88" t="n">
+        <v>2</v>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q88" t="n">
+        <v>284.1</v>
+      </c>
+      <c r="R88" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T88" t="inlineStr"/>
+      <c r="U88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:16:38</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>20</v>
+      </c>
+      <c r="C89" t="n">
+        <v>64</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="H89" t="n">
+        <v>32</v>
+      </c>
+      <c r="I89" t="n">
+        <v>1.2186</v>
+      </c>
+      <c r="J89" t="n">
+        <v>1.2186</v>
+      </c>
+      <c r="K89" t="n">
+        <v>53.1332</v>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N89" t="n">
+        <v>4</v>
+      </c>
+      <c r="O89" t="n">
+        <v>2</v>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q89" t="n">
+        <v>285.3</v>
+      </c>
+      <c r="R89" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T89" t="inlineStr"/>
+      <c r="U89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:16:53</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>20</v>
+      </c>
+      <c r="C90" t="n">
+        <v>64</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="H90" t="n">
+        <v>32</v>
+      </c>
+      <c r="I90" t="n">
+        <v>1.4361</v>
+      </c>
+      <c r="J90" t="n">
+        <v>1.1578</v>
+      </c>
+      <c r="K90" t="n">
+        <v>51.2871</v>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N90" t="n">
+        <v>4</v>
+      </c>
+      <c r="O90" t="n">
+        <v>2</v>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q90" t="n">
+        <v>286.5</v>
+      </c>
+      <c r="R90" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:17:6</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>20</v>
+      </c>
+      <c r="C91" t="n">
+        <v>64</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="H91" t="n">
+        <v>32</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0.9941</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.9941</v>
+      </c>
+      <c r="K91" t="n">
+        <v>53.579</v>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N91" t="n">
+        <v>4</v>
+      </c>
+      <c r="O91" t="n">
+        <v>2</v>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q91" t="n">
+        <v>287.5</v>
+      </c>
+      <c r="R91" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T91" t="inlineStr"/>
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:17:14</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>20</v>
+      </c>
+      <c r="C92" t="n">
+        <v>64</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="H92" t="n">
+        <v>32</v>
+      </c>
+      <c r="I92" t="n">
+        <v>1.4776</v>
+      </c>
+      <c r="J92" t="n">
+        <v>1.1102</v>
+      </c>
+      <c r="K92" t="n">
+        <v>53.6905</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N92" t="n">
+        <v>4</v>
+      </c>
+      <c r="O92" t="n">
+        <v>2</v>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q92" t="n">
+        <v>286.8</v>
+      </c>
+      <c r="R92" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T92" t="inlineStr"/>
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:17:25</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>20</v>
+      </c>
+      <c r="C93" t="n">
+        <v>64</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="H93" t="n">
+        <v>32</v>
+      </c>
+      <c r="I93" t="n">
+        <v>1.1259</v>
+      </c>
+      <c r="J93" t="n">
+        <v>1.1253</v>
+      </c>
+      <c r="K93" t="n">
+        <v>53.1436</v>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N93" t="n">
+        <v>4</v>
+      </c>
+      <c r="O93" t="n">
+        <v>2</v>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q93" t="n">
+        <v>288.8</v>
+      </c>
+      <c r="R93" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T93" t="inlineStr"/>
+      <c r="U93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:17:34</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>20</v>
+      </c>
+      <c r="C94" t="n">
+        <v>64</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="H94" t="n">
+        <v>32</v>
+      </c>
+      <c r="I94" t="n">
+        <v>1.1571</v>
+      </c>
+      <c r="J94" t="n">
+        <v>1.1571</v>
+      </c>
+      <c r="K94" t="n">
+        <v>52.8545</v>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N94" t="n">
+        <v>4</v>
+      </c>
+      <c r="O94" t="n">
+        <v>2</v>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q94" t="n">
+        <v>286.1</v>
+      </c>
+      <c r="R94" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T94" t="inlineStr"/>
+      <c r="U94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:17:39</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>20</v>
+      </c>
+      <c r="C95" t="n">
+        <v>64</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="H95" t="n">
+        <v>32</v>
+      </c>
+      <c r="I95" t="n">
+        <v>1.384</v>
+      </c>
+      <c r="J95" t="n">
+        <v>1.2193</v>
+      </c>
+      <c r="K95" t="n">
+        <v>51.3915</v>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N95" t="n">
+        <v>4</v>
+      </c>
+      <c r="O95" t="n">
+        <v>2</v>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q95" t="n">
+        <v>284.7</v>
+      </c>
+      <c r="R95" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T95" t="inlineStr"/>
+      <c r="U95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:17:51</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>20</v>
+      </c>
+      <c r="C96" t="n">
+        <v>64</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>14.1</v>
+      </c>
+      <c r="H96" t="n">
+        <v>32</v>
+      </c>
+      <c r="I96" t="n">
+        <v>1.1389</v>
+      </c>
+      <c r="J96" t="n">
+        <v>1.1389</v>
+      </c>
+      <c r="K96" t="n">
+        <v>52.6908</v>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>cuda:0</t>
+        </is>
+      </c>
+      <c r="N96" t="n">
+        <v>4</v>
+      </c>
+      <c r="O96" t="n">
+        <v>2</v>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q96" t="n">
+        <v>282</v>
+      </c>
+      <c r="R96" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T96" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="U86" t="n">
+      <c r="U96" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>